<commit_message>
experimental results without normalization for old dataset (ExamDB, Elevator)
</commit_message>
<xml_diff>
--- a/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/Elevator/4wise/0.95_.xlsx
+++ b/experiment_results/20201206_AGGREGATION_AVERAGE_ADDITION_NORMALIZATION3/Elevator/4wise/0.95_.xlsx
@@ -466,34 +466,34 @@
         <v>12</v>
       </c>
       <c r="B2">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="C2">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="D2">
         <v>95</v>
       </c>
       <c r="E2">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F2">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="G2">
         <v>449</v>
       </c>
       <c r="H2">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I2">
         <v>449</v>
       </c>
       <c r="J2">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K2">
-        <v>449</v>
+        <v>374</v>
       </c>
       <c r="L2">
         <v>449</v>
@@ -504,34 +504,34 @@
         <v>13</v>
       </c>
       <c r="B3">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="C3">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="D3">
         <v>55</v>
       </c>
       <c r="E3">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F3">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G3">
         <v>439</v>
       </c>
       <c r="H3">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I3">
         <v>449</v>
       </c>
       <c r="J3">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>432</v>
+        <v>12</v>
       </c>
       <c r="L3">
         <v>449</v>
@@ -542,34 +542,34 @@
         <v>14</v>
       </c>
       <c r="B4">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D4">
         <v>246</v>
       </c>
       <c r="E4">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F4">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G4">
         <v>449</v>
       </c>
       <c r="H4">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I4">
         <v>449</v>
       </c>
       <c r="J4">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K4">
-        <v>449</v>
+        <v>374</v>
       </c>
       <c r="L4">
         <v>449</v>
@@ -580,34 +580,34 @@
         <v>15</v>
       </c>
       <c r="B5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C5">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D5">
         <v>58</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F5">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G5">
         <v>439</v>
       </c>
       <c r="H5">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I5">
         <v>449</v>
       </c>
       <c r="J5">
-        <v>14</v>
+        <v>2</v>
       </c>
       <c r="K5">
-        <v>432</v>
+        <v>12</v>
       </c>
       <c r="L5">
         <v>449</v>
@@ -618,34 +618,34 @@
         <v>16</v>
       </c>
       <c r="B6">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C6">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D6">
         <v>283</v>
       </c>
       <c r="E6">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="F6">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="G6">
         <v>439</v>
       </c>
       <c r="H6">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I6">
         <v>449</v>
       </c>
       <c r="J6">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K6">
-        <v>439</v>
+        <v>22</v>
       </c>
       <c r="L6">
         <v>449</v>
@@ -656,34 +656,34 @@
         <v>17</v>
       </c>
       <c r="B7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="C7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="D7">
         <v>247</v>
       </c>
       <c r="E7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F7">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G7">
         <v>449</v>
       </c>
       <c r="H7">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I7">
         <v>449</v>
       </c>
       <c r="J7">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="K7">
-        <v>449</v>
+        <v>374</v>
       </c>
       <c r="L7">
         <v>449</v>
@@ -694,34 +694,34 @@
         <v>18</v>
       </c>
       <c r="B8">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="C8">
-        <v>-1</v>
+        <v>4</v>
       </c>
       <c r="D8">
         <v>269</v>
       </c>
       <c r="E8">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="F8">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="G8">
         <v>439</v>
       </c>
       <c r="H8">
-        <v>-1</v>
+        <v>5</v>
       </c>
       <c r="I8">
         <v>449</v>
       </c>
       <c r="J8">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K8">
-        <v>439</v>
+        <v>22</v>
       </c>
       <c r="L8">
         <v>449</v>
@@ -732,34 +732,34 @@
         <v>19</v>
       </c>
       <c r="B9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C9">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D9">
         <v>224</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F9">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G9">
         <v>439</v>
       </c>
       <c r="H9">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I9">
         <v>449</v>
       </c>
       <c r="J9">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K9">
-        <v>439</v>
+        <v>22</v>
       </c>
       <c r="L9">
         <v>449</v>
@@ -770,34 +770,34 @@
         <v>20</v>
       </c>
       <c r="B10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D10">
         <v>219</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="G10">
         <v>439</v>
       </c>
       <c r="H10">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="I10">
         <v>449</v>
       </c>
       <c r="J10">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K10">
-        <v>439</v>
+        <v>22</v>
       </c>
       <c r="L10">
         <v>449</v>
@@ -808,34 +808,34 @@
         <v>21</v>
       </c>
       <c r="B11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="C11">
-        <v>-1</v>
+        <v>1</v>
       </c>
       <c r="D11">
         <v>284</v>
       </c>
       <c r="E11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="F11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="G11">
         <v>439</v>
       </c>
       <c r="H11">
-        <v>-1</v>
+        <v>2</v>
       </c>
       <c r="I11">
         <v>449</v>
       </c>
       <c r="J11">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K11">
-        <v>439</v>
+        <v>22</v>
       </c>
       <c r="L11">
         <v>449</v>
@@ -846,34 +846,34 @@
         <v>22</v>
       </c>
       <c r="B12">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="C12">
-        <v>-1</v>
+        <v>15</v>
       </c>
       <c r="D12">
         <v>196</v>
       </c>
       <c r="E12">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="F12">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="G12">
         <v>437</v>
       </c>
       <c r="H12">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="I12">
         <v>449</v>
       </c>
       <c r="J12">
-        <v>15</v>
+        <v>3</v>
       </c>
       <c r="K12">
-        <v>437</v>
+        <v>22</v>
       </c>
       <c r="L12">
         <v>447</v>
@@ -884,34 +884,34 @@
         <v>23</v>
       </c>
       <c r="B13">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="C13">
-        <v>-1</v>
+        <v>3</v>
       </c>
       <c r="D13">
         <v>236</v>
       </c>
       <c r="E13">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="F13">
-        <v>-1</v>
+        <v>8</v>
       </c>
       <c r="G13">
         <v>447</v>
       </c>
       <c r="H13">
-        <v>-1</v>
+        <v>7</v>
       </c>
       <c r="I13">
         <v>449</v>
       </c>
       <c r="J13">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="K13">
-        <v>447</v>
+        <v>380</v>
       </c>
       <c r="L13">
         <v>447</v>

</xml_diff>